<commit_message>
adjusted the excel to refer tot he right datasets
</commit_message>
<xml_diff>
--- a/api/src/main/resources/org/openmrs/module/ugandaemrreports/reports/HMIS_105-2.1-2.7.xlsx
+++ b/api/src/main/resources/org/openmrs/module/ugandaemrreports/reports/HMIS_105-2.1-2.7.xlsx
@@ -56,7 +56,7 @@
     <t>10-19 years</t>
   </si>
   <si>
-    <t>#A1-01#</t>
+    <t>#A.A1-01#</t>
   </si>
   <si>
     <t>E1: Exposed infants tested for HIV below 18 months of age</t>
@@ -68,7 +68,7 @@
     <t>20-24 years</t>
   </si>
   <si>
-    <t>#A1-02#</t>
+    <t>#A.A1-02#</t>
   </si>
   <si>
     <t>2nd PCR</t>
@@ -77,7 +77,7 @@
     <t>&gt;= 25 years</t>
   </si>
   <si>
-    <t>#A1-03#</t>
+    <t>#A.A1-03#</t>
   </si>
   <si>
     <t>&lt; 2 months old</t>
@@ -86,13 +86,13 @@
     <t>No. in 1st Trimester  </t>
   </si>
   <si>
-    <t>#A1-04#</t>
+    <t>#A.A1-04#</t>
   </si>
   <si>
     <t>A2-ANC 4th Visit for women</t>
   </si>
   <si>
-    <t>#A2-01#</t>
+    <t>#A.A2-01#</t>
   </si>
   <si>
     <t>E2: 1st DNA PCR result returned</t>
@@ -101,13 +101,13 @@
     <t>Total</t>
   </si>
   <si>
-    <t>#A2-02#</t>
+    <t>#A.A2-02#</t>
   </si>
   <si>
     <t>HIV+</t>
   </si>
   <si>
-    <t>#A2-03#</t>
+    <t>#A.A2-03#</t>
   </si>
   <si>
     <t>E3: 2nd DNA PCR result returned</t>
@@ -116,22 +116,22 @@
     <t>A3-ANC 4+ visits for Women</t>
   </si>
   <si>
-    <t>#A3#</t>
+    <t>#A.A3#</t>
   </si>
   <si>
     <t>A4- Total ANC visits (newclients+ Re-attendances)</t>
   </si>
   <si>
-    <t>#A4-01#</t>
-  </si>
-  <si>
-    <t>#A4-02#</t>
+    <t>#A.A4-01#</t>
+  </si>
+  <si>
+    <t>#A.A4-02#</t>
   </si>
   <si>
     <t>E4: Number of DNA PCR results returned from the lab</t>
   </si>
   <si>
-    <t>#A4-03#</t>
+    <t>#A.A4-03#</t>
   </si>
   <si>
     <t>Within 2 weeks</t>
@@ -140,7 +140,7 @@
     <t>A5: Referrals to ANC unit</t>
   </si>
   <si>
-    <t>#A5-T#</t>
+    <t>#A.A5-T#</t>
   </si>
   <si>
     <t>Given to caregiver</t>
@@ -149,7 +149,7 @@
     <t>From community services</t>
   </si>
   <si>
-    <t>#A5-CS#</t>
+    <t>#A.A5-CS#</t>
   </si>
   <si>
     <t>E5: Number of HIV Exposed infants tested by serology/rapidHIV test at _x0001_18 months</t>
@@ -158,7 +158,7 @@
     <t>A6-ANC Referrals from unit</t>
   </si>
   <si>
-    <t>#A6-T#</t>
+    <t>#A.A6-T#</t>
   </si>
   <si>
     <t>Positive</t>
@@ -167,7 +167,7 @@
     <t>To FSG</t>
   </si>
   <si>
-    <t>#A6-FSG#</t>
+    <t>#A.A6-FSG#</t>
   </si>
   <si>
     <t>E6: Number of HIV+ infants from EID enrolled in care</t>
@@ -176,19 +176,19 @@
     <t>A7-First dose IPT (IPT1)</t>
   </si>
   <si>
-    <t>#A7-01#</t>
+    <t>#A.A7-01#</t>
   </si>
   <si>
     <t>E7: HIV exposed infants started on CPT</t>
   </si>
   <si>
-    <t>#A7-02#</t>
+    <t>#A.A7-02#</t>
   </si>
   <si>
     <t>Within 2 months</t>
   </si>
   <si>
-    <t>#A7-03#</t>
+    <t>#A.A7-03#</t>
   </si>
   <si>
     <t>2.5 FAMILY PLANNING METHODS</t>
@@ -203,16 +203,16 @@
     <t>A8-Second dose IPT (IPT2</t>
   </si>
   <si>
-    <t>#A8-01#</t>
+    <t>#A.A8-01#</t>
   </si>
   <si>
     <t>F1-Oral : Lo-Femenal</t>
   </si>
   <si>
-    <t>#A8-02#</t>
-  </si>
-  <si>
-    <t>#A8-03#</t>
+    <t>#A.A8-02#</t>
+  </si>
+  <si>
+    <t>#A.A8-03#</t>
   </si>
   <si>
     <t>&gt;=25 years</t>
@@ -221,7 +221,7 @@
     <t>A9-Pregnant Women receiving Iron/Folic Acid on ANC 1st Visit</t>
   </si>
   <si>
-    <t>#A9#</t>
+    <t>#A.A9#</t>
   </si>
   <si>
     <t>F2-Oral: Microgynon</t>
@@ -230,19 +230,19 @@
     <t>A10: Pregnant Women receiving free LLINs</t>
   </si>
   <si>
-    <t>#A10#</t>
+    <t>#A.A10#</t>
   </si>
   <si>
     <t>A11:Pregnant Women tested for syphilis</t>
   </si>
   <si>
-    <t>#A11#</t>
+    <t>#A.A11#</t>
   </si>
   <si>
     <t>A12: Pregnant Women tested positive for syphilis</t>
   </si>
   <si>
-    <t>#A12#</t>
+    <t>#A.A12#</t>
   </si>
   <si>
     <t>F3-Oral: Ovrette oranother POP</t>
@@ -251,13 +251,13 @@
     <t>A13: Pregnant Women newly tested for HIV this pregnancy (TR &amp; TRR)</t>
   </si>
   <si>
-    <t>#A13-01#</t>
-  </si>
-  <si>
-    <t>#A13-02#</t>
-  </si>
-  <si>
-    <t>#A13-03#</t>
+    <t>#A.A13-01#</t>
+  </si>
+  <si>
+    <t>#A.A13-02#</t>
+  </si>
+  <si>
+    <t>#A.A13-03#</t>
   </si>
   <si>
     <t>F4-Oral: Others</t>
@@ -266,13 +266,13 @@
     <t>A14: Pregnant Women tested HIV+ for 1st time this pregnancy (TRR) at any visit</t>
   </si>
   <si>
-    <t>#A14-01#</t>
-  </si>
-  <si>
-    <t>#A14-02#</t>
-  </si>
-  <si>
-    <t>#A14-03#</t>
+    <t>#A.A14-01#</t>
+  </si>
+  <si>
+    <t>#A.A14-02#</t>
+  </si>
+  <si>
+    <t>#A.A14-03#</t>
   </si>
   <si>
     <t>F5-Female condoms</t>
@@ -284,19 +284,19 @@
     <t>CD4</t>
   </si>
   <si>
-    <t>#A15-CD4#</t>
+    <t>#A.A15-CD4#</t>
   </si>
   <si>
     <t>WHO clinical stage only</t>
   </si>
   <si>
-    <t>#A15-WHO#</t>
+    <t>#A.A15-WHO#</t>
   </si>
   <si>
     <t>A16: HIV+ Pregnant Women initiated on ART for EMTCT (ART)</t>
   </si>
   <si>
-    <t>#A16#</t>
+    <t>#A.A16#</t>
   </si>
   <si>
     <t>F6-Male condoms</t>
@@ -308,19 +308,19 @@
     <t>Total (TRK + TRRK)</t>
   </si>
   <si>
-    <t>#A17-T#</t>
+    <t>#A.A17-T#</t>
   </si>
   <si>
     <t>HIV+ (TRRK)</t>
   </si>
   <si>
-    <t>#A17-TRRk#</t>
+    <t>#A.A17-TRRk#</t>
   </si>
   <si>
     <t>A18: HIV+ Pregnant Women already on ART before 1st ANC (ART-K)</t>
   </si>
   <si>
-    <t>#A18#</t>
+    <t>#A.A18#</t>
   </si>
   <si>
     <t>F7-IUDs</t>
@@ -329,19 +329,19 @@
     <t>A19: Pregnant Women re-tested later in pregnancy (TR+&amp;TRR+)</t>
   </si>
   <si>
-    <t>#A19#</t>
+    <t>#A.A19#</t>
   </si>
   <si>
     <t>A20: Pregnant Women testing HIV+ on a retest (TRR+)</t>
   </si>
   <si>
-    <t>#A20#</t>
+    <t>#A.A20#</t>
   </si>
   <si>
     <t>A21: HIV+ Pregnant Women initiated on Cotrimoxazole</t>
   </si>
   <si>
-    <t>#A21#</t>
+    <t>#A.A21#</t>
   </si>
   <si>
     <t>F8-Injectable</t>
@@ -350,10 +350,10 @@
     <t>A22: Male partners received HIV test results in eMTCT</t>
   </si>
   <si>
-    <t>#A22-T#</t>
-  </si>
-  <si>
-    <t>#A22-HIVp#</t>
+    <t>#A.A22-T#</t>
+  </si>
+  <si>
+    <t>#A.A22-HIVp#</t>
   </si>
   <si>
     <t>2.2 MATERNITY</t>
@@ -545,37 +545,37 @@
     <t>P1-Post Natal Attendances</t>
   </si>
   <si>
-    <t>#P1-A-01#</t>
-  </si>
-  <si>
-    <t>#P1-A-02#</t>
-  </si>
-  <si>
-    <t>#P1-A-03#</t>
+    <t>#P.P1-A-01#</t>
+  </si>
+  <si>
+    <t>#P.P1-A-02#</t>
+  </si>
+  <si>
+    <t>#P.P1-A-03#</t>
   </si>
   <si>
     <t>6 Hours</t>
   </si>
   <si>
-    <t>#P1-6H#</t>
+    <t>#P.P1-6H#</t>
   </si>
   <si>
     <t>6 Days</t>
   </si>
   <si>
-    <t>#P1-6D#</t>
+    <t>#P.P1-6D#</t>
   </si>
   <si>
     <t>6 Weeks</t>
   </si>
   <si>
-    <t>#P1-6W#</t>
+    <t>#P.P1-6W#</t>
   </si>
   <si>
     <t>6 Months</t>
   </si>
   <si>
-    <t>#P1-6M#</t>
+    <t>#P.P1-6M#</t>
   </si>
   <si>
     <t>P2: Breastfeeding mothers tested for HIV</t>
@@ -584,58 +584,58 @@
     <t>1st test during Postnatal</t>
   </si>
   <si>
-    <t>#P2-1#</t>
+    <t>#P.P2-1#</t>
   </si>
   <si>
     <t>Retest during Postnatal</t>
   </si>
   <si>
-    <t>#P2-2#</t>
+    <t>#P.P2-2#</t>
   </si>
   <si>
     <t>P3: Breastfeeding mothers newly testingHIV+</t>
   </si>
   <si>
-    <t>#P3-1#</t>
-  </si>
-  <si>
-    <t>#P3-2#</t>
+    <t>#P.P3-1#</t>
+  </si>
+  <si>
+    <t>#P.P3-2#</t>
   </si>
   <si>
     <t>P4: Total HIV+ mothers attending postnatal</t>
   </si>
   <si>
-    <t>#P4#</t>
+    <t>#P.P4#</t>
   </si>
   <si>
     <t>P5: HIV+ women initiating ART in PNC</t>
   </si>
   <si>
-    <t>#P5#</t>
+    <t>#P.P5#</t>
   </si>
   <si>
     <t>P6: Mother-baby pairs enrolled at Mother-Baby care point</t>
   </si>
   <si>
-    <t>#P6#</t>
+    <t>#P.P6#</t>
   </si>
   <si>
     <t>P7: Vitamin A supplementation given to mothers</t>
   </si>
   <si>
-    <t>#P7#</t>
+    <t>#P.P7#</t>
   </si>
   <si>
     <t>P8: Clients with pre-malignant conditions of breast</t>
   </si>
   <si>
-    <t>#P8#</t>
+    <t>#P.P8#</t>
   </si>
   <si>
     <t>P9: Clients with pre-malignant conditions of cervix</t>
   </si>
   <si>
-    <t>#P9#</t>
+    <t>#P.P9#</t>
   </si>
 </sst>
 </file>
@@ -645,7 +645,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="GENERAL"/>
   </numFmts>
-  <fonts count="6">
+  <fonts count="5">
     <font>
       <sz val="12"/>
       <name val="Calibri"/>
@@ -673,11 +673,6 @@
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <name val="Calibri"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="3">
@@ -749,7 +744,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="18">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -819,10 +814,6 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -905,8 +896,8 @@
   </sheetPr>
   <dimension ref="A1:L105"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A91" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D105" activeCellId="0" sqref="D105"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A34" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D49" activeCellId="0" sqref="D49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75"/>
@@ -1092,6 +1083,7 @@
       <c r="L9" s="0"/>
     </row>
     <row r="10" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A10" s="0"/>
       <c r="B10" s="7" t="s">
         <v>22</v>
       </c>
@@ -1100,8 +1092,10 @@
         <v>23</v>
       </c>
       <c r="E10" s="6"/>
+      <c r="F10" s="0"/>
       <c r="G10" s="7"/>
       <c r="H10" s="7"/>
+      <c r="I10" s="0"/>
       <c r="J10" s="0"/>
       <c r="K10" s="0"/>
       <c r="L10" s="0"/>
@@ -1185,6 +1179,7 @@
       <c r="F14" s="6"/>
       <c r="G14" s="7"/>
       <c r="H14" s="7"/>
+      <c r="I14" s="0"/>
       <c r="J14" s="0"/>
       <c r="K14" s="0"/>
       <c r="L14" s="0"/>
@@ -2519,6 +2514,7 @@
       <c r="A83" s="4"/>
       <c r="B83" s="4"/>
       <c r="C83" s="4"/>
+      <c r="D83" s="0"/>
     </row>
     <row r="84" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A84" s="4" t="s">
@@ -2716,7 +2712,7 @@
       </c>
       <c r="B103" s="4"/>
       <c r="C103" s="4"/>
-      <c r="D103" s="18" t="s">
+      <c r="D103" s="2" t="s">
         <v>202</v>
       </c>
     </row>

</xml_diff>